<commit_message>
Added timers, comments and stats
</commit_message>
<xml_diff>
--- a/Nomic.xlsx
+++ b/Nomic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Nomic-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A9C4A7-A596-4F27-BF27-A78CBCFB0FC3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C96794A-AA2E-45B7-BFD9-41CD1446C83A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,23 +22,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Player Display Name</t>
   </si>
   <si>
-    <t>ZgH</t>
-  </si>
-  <si>
     <t>Player Username</t>
   </si>
   <si>
     <t>Player ID</t>
   </si>
   <si>
-    <t>259220635010596864</t>
-  </si>
-  <si>
     <t>Still Playing?</t>
   </si>
   <si>
@@ -81,10 +75,22 @@
     <t>Current Votes</t>
   </si>
   <si>
+    <t>Empty?</t>
+  </si>
+  <si>
     <t>Stat Rows</t>
   </si>
   <si>
-    <t>Empty?</t>
+    <t>Proposal Time</t>
+  </si>
+  <si>
+    <t>Voting Time</t>
+  </si>
+  <si>
+    <t>Yes Proportion</t>
+  </si>
+  <si>
+    <t>Current Logins</t>
   </si>
 </sst>
 </file>
@@ -447,7 +453,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,76 +467,60 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1"/>
     </row>
     <row r="2" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="B2"/>
     </row>
     <row r="3" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B3"/>
     </row>
     <row r="4" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
     </row>
     <row r="5" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B5"/>
     </row>
     <row r="6" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B8"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B9"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B10"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -542,7 +532,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -556,42 +546,31 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="4" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="A4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+    </row>
     <row r="6" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -600,10 +579,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -613,15 +592,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -629,39 +608,71 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B14">
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
         <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ready to start game (?)
</commit_message>
<xml_diff>
--- a/Nomic.xlsx
+++ b/Nomic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Nomic-Bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bots\Nomic-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C96794A-AA2E-45B7-BFD9-41CD1446C83A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8DA747-583F-4895-867C-488B190052B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Player Display Name</t>
   </si>
@@ -33,9 +33,18 @@
     <t>Player ID</t>
   </si>
   <si>
+    <t>Points</t>
+  </si>
+  <si>
     <t>Still Playing?</t>
   </si>
   <si>
+    <t>Current Vote</t>
+  </si>
+  <si>
+    <t>Daily Login</t>
+  </si>
+  <si>
     <t>Stats</t>
   </si>
   <si>
@@ -51,6 +60,12 @@
     <t>Total Proposals</t>
   </si>
   <si>
+    <t>Total First Votes</t>
+  </si>
+  <si>
+    <t>Total Deciding Votes</t>
+  </si>
+  <si>
     <t>Turn</t>
   </si>
   <si>
@@ -63,6 +78,9 @@
     <t>Passed?</t>
   </si>
   <si>
+    <t>End Con</t>
+  </si>
+  <si>
     <t>Player Number</t>
   </si>
   <si>
@@ -72,13 +90,10 @@
     <t>State</t>
   </si>
   <si>
-    <t>Current Votes</t>
-  </si>
-  <si>
-    <t>Empty?</t>
-  </si>
-  <si>
-    <t>Stat Rows</t>
+    <t>First Vote</t>
+  </si>
+  <si>
+    <t>Last Vote</t>
   </si>
   <si>
     <t>Proposal Time</t>
@@ -88,9 +103,6 @@
   </si>
   <si>
     <t>Yes Proportion</t>
-  </si>
-  <si>
-    <t>Current Logins</t>
   </si>
 </sst>
 </file>
@@ -450,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,41 +498,69 @@
     </row>
     <row r="5" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5"/>
+    </row>
+    <row r="6" spans="1:2" s="4" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5"/>
-    </row>
-    <row r="6" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="B8"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="9" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B10"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -529,49 +569,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-    </row>
-    <row r="5" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-    </row>
-    <row r="6" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+    </row>
+    <row r="4" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J12" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -579,10 +630,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -592,7 +643,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -600,7 +651,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -608,70 +659,55 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>86400</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13">
         <v>86400</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14">
-        <v>86400</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Why was that even a bug
</commit_message>
<xml_diff>
--- a/Nomic.xlsx
+++ b/Nomic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bots\Nomic-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8DA747-583F-4895-867C-488B190052B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F50C67-2355-4568-82E0-66799C131BAE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="2580" windowWidth="17280" windowHeight="9420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
@@ -633,7 +633,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -662,7 +662,7 @@
         <v>20</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Start of round 2
</commit_message>
<xml_diff>
--- a/Nomic.xlsx
+++ b/Nomic.xlsx
@@ -143,16 +143,18 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -453,42 +455,39 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" style="1" width="20.109375"/>
-    <col customWidth="1" max="4" min="2" style="4" width="12.109375"/>
-    <col customWidth="1" max="9" min="5" style="4" width="12.109375"/>
-    <col customWidth="1" max="10" min="10" style="4" width="12.109375"/>
-    <col customWidth="1" max="20" min="11" style="4" width="12.109375"/>
+    <col customWidth="1" max="20" min="2" style="4" width="12.109375"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="15.6" r="1" s="4">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>Player Display Name</t>
+          <t>Player Name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>HummingBee | Aria | She/Her</t>
+          <t>HummingBee</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Zac</t>
+          <t>Kiwi</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Wice || Petew uwu</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Outgwid | she/her</t>
+          <t>Outgrid</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -498,47 +497,47 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>ToasterB | Joseph</t>
+          <t>ToasterB</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Steven</t>
+          <t>Sevnet</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Xiong_D_Kuma</t>
+          <t>Kuma</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>UndeathMetal | He/They</t>
+          <t>UndeathMetal</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Mentawist | Bhawgava</t>
+          <t>Mentalist</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>Lipton</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>Sam</t>
+          <t>Thunderbird</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>realcateye | Cat</t>
+          <t>Realcateye</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>Travesty | He/They</t>
+          <t>Travesty</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
@@ -548,22 +547,22 @@
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>HappyNewYeesh || Ayeesha</t>
+          <t>Yeesh</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>Sheepish | Emily</t>
+          <t>Sheepish</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>King Platapus | Nathan</t>
+          <t>King Platapus</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>Melo | she/her</t>
+          <t>Melo</t>
         </is>
       </c>
     </row>
@@ -640,7 +639,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>PARTYPOISON</t>
+          <t>wayward</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -805,7 +804,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="b">
         <v>1</v>
@@ -844,62 +843,62 @@
           <t>Last Message</t>
         </is>
       </c>
-      <c r="B6" s="16" t="n">
-        <v>43922.79375396144</v>
-      </c>
-      <c r="C6" s="16" t="n">
-        <v>43922.50591435185</v>
-      </c>
-      <c r="D6" s="16" t="n">
-        <v>43922.59549768519</v>
-      </c>
-      <c r="E6" s="16" t="n">
-        <v>43922.61008101852</v>
-      </c>
-      <c r="F6" s="16" t="n">
-        <v>43922.53508101852</v>
-      </c>
-      <c r="G6" s="16" t="n">
-        <v>43922.53230324074</v>
-      </c>
-      <c r="H6" s="16" t="n">
-        <v>43922.50591435185</v>
-      </c>
-      <c r="I6" s="16" t="n">
+      <c r="B6" s="13" t="n">
+        <v>43931.08071832073</v>
+      </c>
+      <c r="C6" s="13" t="n">
+        <v>43930.73059961732</v>
+      </c>
+      <c r="D6" s="13" t="n">
+        <v>43930.7838577714</v>
+      </c>
+      <c r="E6" s="13" t="n">
+        <v>43930.76625446408</v>
+      </c>
+      <c r="F6" s="13" t="n">
+        <v>43930.7834052686</v>
+      </c>
+      <c r="G6" s="13" t="n">
+        <v>43930.76401516177</v>
+      </c>
+      <c r="H6" s="13" t="n">
+        <v>43928.83637651578</v>
+      </c>
+      <c r="I6" s="13" t="n">
         <v>43922.59758101852</v>
       </c>
-      <c r="J6" s="16" t="n">
-        <v>43922.52605324074</v>
-      </c>
-      <c r="K6" s="16" t="n">
-        <v>43922.58369212963</v>
-      </c>
-      <c r="L6" s="16" t="n">
-        <v>43922.58230324074</v>
-      </c>
-      <c r="M6" s="16" t="n">
-        <v>43922.54063657407</v>
-      </c>
-      <c r="N6" s="16" t="n">
-        <v>43922.75610113703</v>
-      </c>
-      <c r="O6" s="16" t="n">
-        <v>43922.76207976044</v>
-      </c>
-      <c r="P6" s="16" t="n">
+      <c r="J6" s="13" t="n">
+        <v>43930.83546035166</v>
+      </c>
+      <c r="K6" s="13" t="n">
+        <v>43930.73022517501</v>
+      </c>
+      <c r="L6" s="13" t="n">
+        <v>43930.77580448762</v>
+      </c>
+      <c r="M6" s="13" t="n">
+        <v>43930.82408426917</v>
+      </c>
+      <c r="N6" s="13" t="n">
+        <v>43930.73400248589</v>
+      </c>
+      <c r="O6" s="13" t="n">
+        <v>43929.74655898</v>
+      </c>
+      <c r="P6" s="13" t="n">
         <v>43917.74341435185</v>
       </c>
-      <c r="Q6" s="16" t="n">
-        <v>43922.51563657408</v>
-      </c>
-      <c r="R6" s="16" t="n">
-        <v>43922.5066087963</v>
-      </c>
-      <c r="S6" s="16" t="n">
-        <v>43922.59271990741</v>
-      </c>
-      <c r="T6" s="16" t="n">
-        <v>43921.87674768519</v>
+      <c r="Q6" s="13" t="n">
+        <v>43930.73045180638</v>
+      </c>
+      <c r="R6" s="13" t="n">
+        <v>43930.75334761043</v>
+      </c>
+      <c r="S6" s="13" t="n">
+        <v>43929.76516309773</v>
+      </c>
+      <c r="T6" s="13" t="n">
+        <v>43930.76725111798</v>
       </c>
     </row>
     <row customHeight="1" ht="15.6" r="7" s="4">
@@ -933,13 +932,13 @@
         <v>5</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -960,7 +959,7 @@
         <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
@@ -984,43 +983,43 @@
         <v>1</v>
       </c>
       <c r="C9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" t="b">
         <v>0</v>
       </c>
       <c r="N9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P9" t="b">
         <v>0</v>
@@ -1032,7 +1031,7 @@
         <v>0</v>
       </c>
       <c r="S9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T9" t="b">
         <v>0</v>
@@ -1055,22 +1054,22 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>202</v>
+        <v>688</v>
       </c>
       <c r="C12" t="n">
-        <v>23</v>
+        <v>211</v>
       </c>
       <c r="D12" t="n">
-        <v>113</v>
+        <v>214</v>
       </c>
       <c r="E12" t="n">
-        <v>104</v>
+        <v>199</v>
       </c>
       <c r="F12" t="n">
-        <v>96</v>
+        <v>301</v>
       </c>
       <c r="G12" t="n">
-        <v>102</v>
+        <v>319</v>
       </c>
       <c r="H12" t="n">
         <v>6</v>
@@ -1079,37 +1078,37 @@
         <v>7</v>
       </c>
       <c r="J12" t="n">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="K12" t="n">
-        <v>54</v>
+        <v>363</v>
       </c>
       <c r="L12" t="n">
-        <v>68</v>
+        <v>393</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N12" t="n">
-        <v>4</v>
+        <v>179</v>
       </c>
       <c r="O12" t="n">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="P12" t="n">
         <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="R12" t="n">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="S12" t="n">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="T12" t="n">
-        <v>14</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13">
@@ -1119,61 +1118,61 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I13" t="n">
         <v>2</v>
       </c>
       <c r="J13" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="N13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="O13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="P13" t="n">
         <v>2</v>
       </c>
       <c r="Q13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="R13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="S13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="T13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -1183,61 +1182,61 @@
         </is>
       </c>
       <c r="B14" t="n">
+        <v>10</v>
+      </c>
+      <c r="C14" t="n">
+        <v>10</v>
+      </c>
+      <c r="D14" t="n">
+        <v>8</v>
+      </c>
+      <c r="E14" t="n">
+        <v>8</v>
+      </c>
+      <c r="F14" t="n">
+        <v>9</v>
+      </c>
+      <c r="G14" t="n">
+        <v>9</v>
+      </c>
+      <c r="H14" t="n">
         <v>2</v>
       </c>
-      <c r="C14" t="n">
+      <c r="I14" t="n">
+        <v>3</v>
+      </c>
+      <c r="J14" t="n">
+        <v>5</v>
+      </c>
+      <c r="K14" t="n">
+        <v>9</v>
+      </c>
+      <c r="L14" t="n">
+        <v>10</v>
+      </c>
+      <c r="M14" t="n">
         <v>2</v>
       </c>
-      <c r="D14" t="n">
+      <c r="N14" t="n">
+        <v>6</v>
+      </c>
+      <c r="O14" t="n">
+        <v>7</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
         <v>2</v>
       </c>
-      <c r="E14" t="n">
-        <v>2</v>
-      </c>
-      <c r="F14" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" t="n">
-        <v>2</v>
-      </c>
-      <c r="H14" t="n">
-        <v>1</v>
-      </c>
-      <c r="I14" t="n">
-        <v>2</v>
-      </c>
-      <c r="J14" t="n">
-        <v>2</v>
-      </c>
-      <c r="K14" t="n">
-        <v>2</v>
-      </c>
-      <c r="L14" t="n">
-        <v>2</v>
-      </c>
-      <c r="M14" t="n">
-        <v>1</v>
-      </c>
-      <c r="N14" t="n">
-        <v>1</v>
-      </c>
-      <c r="O14" t="n">
-        <v>2</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>1</v>
-      </c>
       <c r="R14" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S14" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="T14" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
@@ -1271,22 +1270,22 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P15" t="n">
         <v>0</v>
@@ -1295,13 +1294,13 @@
         <v>0</v>
       </c>
       <c r="R15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -1311,22 +1310,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1338,10 +1337,10 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M16" t="n">
         <v>0</v>
@@ -1375,7 +1374,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -1384,7 +1383,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -1393,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" t="n">
         <v>1</v>
@@ -1402,13 +1401,13 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N17" t="n">
         <v>0</v>
@@ -1433,7 +1432,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="15" t="n"/>
+      <c r="B20" s="12" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1446,10 +1445,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:X19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6" outlineLevelCol="0"/>
@@ -1464,27 +1463,27 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>Player Display Name</t>
+          <t>Player Name</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>HummingBee | Aria | She/Her</t>
+          <t>HummingBee</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Zac</t>
+          <t>Kiwi</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Wice || Petew uwu</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Outgwid | she/her</t>
+          <t>Outgrid</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
@@ -1494,47 +1493,47 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>ToasterB | Joseph</t>
+          <t>ToasterB</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>Steven</t>
+          <t>Sevnet</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>Xiong_D_Kuma</t>
+          <t>Kuma</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>UndeathMetal | He/They</t>
+          <t>UndeathMetal</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>Mentawist | Bhawgava</t>
+          <t>Mentalist</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>Lipton</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>Sam</t>
+          <t>Thunderbird</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>realcateye | Cat</t>
+          <t>Realcateye</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>Travesty | He/They</t>
+          <t>Travesty</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
@@ -1544,22 +1543,22 @@
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>HappyNewYeesh || Ayeesha</t>
+          <t>Yeesh</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>Sheepish | Emily</t>
+          <t>Sheepish</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>King Platapus | Nathan</t>
+          <t>King Platapus</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>Melo | she/her</t>
+          <t>Melo</t>
         </is>
       </c>
     </row>
@@ -1601,7 +1600,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HummingBee | Aria | She/Her</t>
+          <t>HummingBee</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -1717,7 +1716,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Zac</t>
+          <t>Kiwi</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -1833,7 +1832,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Wice || Petew uwu</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1949,7 +1948,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Outgwid | she/her</t>
+          <t>Outgrid</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -2181,7 +2180,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ToasterB | Joseph</t>
+          <t>ToasterB</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -2297,7 +2296,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Steven</t>
+          <t>Sevnet</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -2403,13 +2402,1069 @@
       </c>
     </row>
     <row r="10">
-      <c r="K10" s="2" t="n"/>
+      <c r="A10" t="n">
+        <v>7</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>385682387511541760</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>UndeathMetal</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="K10" s="2" t="inlineStr">
+        <is>
+          <t>1,0</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>1,1</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>2,2</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="K11" s="2" t="n"/>
+      <c r="A11" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>226145506730967051</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Mentalist</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>1,2</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1,9</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>1,6</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>1,0</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>2,12</t>
+        </is>
+      </c>
+      <c r="K11" s="2" t="inlineStr">
+        <is>
+          <t>1,1</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>1,7</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>1,13</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>1,15</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>2,11</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>1,14</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>1,3</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>1,8</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>1,4</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>1,5</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>2,10</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="K12" s="2" t="n"/>
+      <c r="A12" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>254489242263093248</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Lipton</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2,2</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2,0</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2,4</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
+          <t>2,1</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>1,0</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>2,3</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="14.4" r="13" s="4">
+      <c r="A13" t="n">
+        <v>10</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>280617649300570123</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Thunderbird</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>1,0</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1,9</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>1,5</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>1,12</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>1,1</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>1,10</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>1,11</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>1,2</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>1,3</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>1,8</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>1,7</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>1,4</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>1,6</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="14.4" r="14" s="4">
+      <c r="A14" t="n">
+        <v>11</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>688665453546962964</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Realcateye</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2,7</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1,1</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>2,6</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>2,4</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>2,5</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>2,0</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>1,3</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>1,2</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="14.4" r="15" s="4">
+      <c r="A15" t="n">
+        <v>12</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>620180291197075467</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Travesty</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>1,2</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1,3</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>1,7</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>1,8</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>1,9</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>1,10</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>1,0</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>1,12</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>1,11</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>1,1</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>1,6</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>1,4</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>1,5</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>692264423406174289</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Yeesh</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="14.4" r="17" s="4">
+      <c r="A17" t="n">
+        <v>14</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>115900946722193409</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Sheepish</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>1,1</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1,9</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>1,6</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>1,5</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>1,10</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>1,0</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>1,11</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>1,4</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>2,12</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>1,2</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>1,8</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>1,11</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>1,3</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>1,7</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="14.4" r="18" s="4">
+      <c r="A18" t="n">
+        <v>15</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>162427580031434752</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>King Platapus</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1,1</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>1,6</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2,3</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>2,7</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>2,8</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>2,0</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>2,4</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>1,2</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>1,5</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="14.4" r="19" s="4">
+      <c r="A19" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>170430609716543490</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Melo</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>1,1</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>1,4</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>1,6</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>1,11</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>1,8</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>1,10</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>1,2</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>1,0</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>1,12</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>1,7</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>-2,</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>1,3</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>1,9</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>0,</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>1,5</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -2423,10 +3478,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6" outlineLevelCol="0"/>
@@ -2451,7 +3506,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2461,7 +3516,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
@@ -2527,7 +3582,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.75,1</t>
+          <t>0.75,0.85</t>
         </is>
       </c>
     </row>
@@ -2539,7 +3594,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0.75,1</t>
+          <t>0.75,0.85</t>
         </is>
       </c>
     </row>
@@ -2551,7 +3606,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0,1</t>
+          <t>0,0</t>
         </is>
       </c>
     </row>
@@ -2562,7 +3617,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -2571,12 +3626,22 @@
           <t>TimerEnd</t>
         </is>
       </c>
-      <c r="B17" s="15" t="n">
-        <v>43923.6410480011</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
+      <c r="B17" s="12" t="n">
+        <v>43931.82445956271</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>Ready</t>
+        </is>
+      </c>
+      <c r="B18" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
         <is>
           <t>SummaryMsgID</t>
         </is>
@@ -2593,10 +3658,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="O49" sqref="O49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
@@ -3003,7 +4068,7 @@
       </c>
     </row>
     <row customHeight="1" ht="409.6" r="34" s="4">
-      <c r="A34" s="12" t="n">
+      <c r="A34" s="14" t="n">
         <v>304</v>
       </c>
       <c r="B34" s="10" t="inlineStr">
@@ -3020,18 +4085,45 @@
       </c>
     </row>
     <row customHeight="1" ht="198.6" r="35" s="4">
-      <c r="A35" s="12" t="n">
+      <c r="A35" s="14" t="n">
         <v>306</v>
       </c>
-      <c r="B35" s="14" t="inlineStr">
+      <c r="B35" s="11" t="inlineStr">
         <is>
           <t>Title: Inactivity
 If any player has failed to vote in 3 consecutive proposals AND at least 72 hours have passed since the player last posted a message to the discord server (in any channel), their @player role must be removed and replaced by the @inactiveplayer role by the historian. Any player may voluntarily remove their @player role and replace it with the @inactiveplayer role by using the ~cryosleep command in the #bot-commands channel. Anyone with the @inactiveplayer role retains their slot in the turn order, but if the turn would be passed to them they are skipped and the turn is passed to the player immediately following them in the turn order. Anyone with the @inactiveplayer role may use the ~resurrect command in the #bot-commands channel to replace their @inactiveplayer role with an @player role at any time. Any other action taken by anyone with the @inactiveplayer role is wholly null and void. Anyone with the @inactiveplayer role must comply with this rule.</t>
         </is>
       </c>
     </row>
-    <row r="36">
-      <c r="B36" s="13" t="n"/>
+    <row customHeight="1" ht="93" r="36" s="4">
+      <c r="A36" s="14" t="n">
+        <v>309</v>
+      </c>
+      <c r="B36" s="16" t="inlineStr">
+        <is>
+          <t>Title: Democracy
+This rule takes precedence over rules 204 and 206. 
+Points cannot be gained as a result of:
+1. Making proposals
+2. Having your proposals succeed or fail
+3. Voting yes or no on proposals</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" s="15" t="n"/>
+    </row>
+    <row r="39">
+      <c r="B39" s="15" t="n"/>
+    </row>
+    <row r="40">
+      <c r="B40" s="15" t="n"/>
+    </row>
+    <row r="41">
+      <c r="B41" s="15" t="n"/>
+    </row>
+    <row r="42">
+      <c r="B42" s="15" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>